<commit_message>
Several, testing conditions on dashboard
</commit_message>
<xml_diff>
--- a/seed_data.xlsx
+++ b/seed_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -89,19 +89,70 @@
     <t xml:space="preserve">Issue security lockdown</t>
   </si>
   <si>
+    <t xml:space="preserve">clear_method</t>
+  </si>
+  <si>
     <t xml:space="preserve">effect</t>
   </si>
   <si>
     <t xml:space="preserve">Exhausted </t>
   </si>
   <si>
-    <t xml:space="preserve">Disadvantage on physical tasks until rested. </t>
+    <t xml:space="preserve">You are exhausted, impairing your capabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rest:3, Stimulant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skill:0.95</t>
   </si>
   <si>
     <t xml:space="preserve">Injured </t>
   </si>
   <si>
-    <t xml:space="preserve">Cannot take physical actions without assistance. </t>
+    <t xml:space="preserve">You are hurt. Cannot take physical actions without assistance. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skill:0.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical Injury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are severely injured. Perform no further actions and seek medical attention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skill:0.00, Knowledge:0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypoxia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are in a low oxygen environment, impairing your cognitive functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skill:0.75, Knowledge:0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neural Jack Virus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your augments have been infected with a virus that disrupts your Neural Jack Connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability Restriction:neural jack</t>
   </si>
   <si>
     <t xml:space="preserve">location</t>
@@ -135,9 +186,6 @@
   </si>
   <si>
     <t xml:space="preserve">control@redshift.local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Control</t>
   </si>
   <si>
     <t xml:space="preserve">Susan</t>
@@ -550,10 +598,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -566,23 +614,83 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -614,16 +722,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -652,30 +760,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>36</v>
@@ -683,30 +791,30 @@
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -741,169 +849,169 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,60 +1083,60 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1049,7 +1157,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1057,16 +1165,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1074,13 +1182,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>